<commit_message>
Mixer2 - BOM wip
</commit_message>
<xml_diff>
--- a/modules/Mixer2/Mixer2-BOM.xlsx
+++ b/modules/Mixer2/Mixer2-BOM.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,24 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\Mixer2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{AA834781-FFF1-4AEF-A7FF-1435CF768BAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC75884-C439-4C60-907E-73F25282B821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6465" yWindow="1350" windowWidth="19110" windowHeight="10695"/>
+    <workbookView xWindow="6465" yWindow="1350" windowWidth="19110" windowHeight="10695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mixer2-BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Len P</author>
   </authors>
   <commentList>
-    <comment ref="B24" authorId="0" shapeId="0">
+    <comment ref="B22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -34,7 +46,8 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>D-shaft for small knobs</t>
+          <t>D-shaft for small knobs.
+Also need more knobs!</t>
         </r>
       </text>
     </comment>
@@ -43,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="176">
   <si>
     <t>Ref</t>
   </si>
@@ -339,12 +352,6 @@
     <t>https://www.adafruit.com/product/4031</t>
   </si>
   <si>
-    <t>J9</t>
-  </si>
-  <si>
-    <t>Conn_Front_Left_Top</t>
-  </si>
-  <si>
     <t>Generic connector, single row, 01x09, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
@@ -357,12 +364,6 @@
     <t>https://www.mouser.ca/ProductDetail/Wurth-Elektronik/61303211821?qs=ZtY9WdtwX55M%2FH%2FSrHZ9xA%3D%3D</t>
   </si>
   <si>
-    <t>J10</t>
-  </si>
-  <si>
-    <t>Conn_Back_Right_Top</t>
-  </si>
-  <si>
     <t>https://www.adafruit.com/product/392</t>
   </si>
   <si>
@@ -372,18 +373,6 @@
     <t>https://www.mouser.ca/ProductDetail/649-1012937893601BLF</t>
   </si>
   <si>
-    <t>J11</t>
-  </si>
-  <si>
-    <t>Conn_Front_Right</t>
-  </si>
-  <si>
-    <t>J12</t>
-  </si>
-  <si>
-    <t>Conn_Back_Left</t>
-  </si>
-  <si>
     <t>J13</t>
   </si>
   <si>
@@ -583,12 +572,24 @@
   </si>
   <si>
     <t>Need</t>
+  </si>
+  <si>
+    <t>Conn_PCB_Front</t>
+  </si>
+  <si>
+    <t>J9 J11</t>
+  </si>
+  <si>
+    <t>Conn_PCB_Back</t>
+  </si>
+  <si>
+    <t>J10 J12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1142,10 +1143,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1444,11 +1441,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1465,13 +1462,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -1529,9 +1526,12 @@
       <c r="B2">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
       <c r="E2">
         <f>MAX(0,B2-C2-D2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="s">
         <v>19</v>
@@ -1569,7 +1569,7 @@
         <v>2</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E26" si="0">MAX(0,B3-C3-D3)</f>
+        <f t="shared" ref="E3:E24" si="0">MAX(0,B3-C3-D3)</f>
         <v>2</v>
       </c>
       <c r="F3" t="s">
@@ -1763,9 +1763,12 @@
       <c r="B8">
         <v>4</v>
       </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F8" t="s">
         <v>74</v>
@@ -1781,9 +1784,12 @@
       <c r="B9">
         <v>2</v>
       </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F9" t="s">
         <v>77</v>
@@ -1826,9 +1832,12 @@
       <c r="B10">
         <v>8</v>
       </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F10" t="s">
         <v>87</v>
@@ -1875,20 +1884,23 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>98</v>
+        <v>173</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>99</v>
+        <v>172</v>
       </c>
       <c r="I11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="M11" t="s">
         <v>96</v>
@@ -1897,34 +1909,37 @@
         <v>598</v>
       </c>
       <c r="O11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="P11" t="s">
         <v>35</v>
       </c>
       <c r="Q11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="R11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>104</v>
+        <v>175</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>105</v>
+        <v>174</v>
       </c>
       <c r="I12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="M12" t="s">
         <v>96</v>
@@ -1933,177 +1948,189 @@
         <v>392</v>
       </c>
       <c r="O12" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="P12" t="s">
         <v>35</v>
       </c>
       <c r="Q12" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="R12" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" t="s">
+        <v>106</v>
+      </c>
+      <c r="I13" t="s">
+        <v>107</v>
+      </c>
+      <c r="J13" t="s">
+        <v>108</v>
+      </c>
+      <c r="K13" t="s">
+        <v>109</v>
+      </c>
+      <c r="L13">
+        <v>61201021621</v>
+      </c>
+      <c r="M13" t="s">
+        <v>35</v>
+      </c>
+      <c r="N13" t="s">
         <v>110</v>
       </c>
-      <c r="I13" t="s">
-        <v>100</v>
-      </c>
-      <c r="M13" t="s">
-        <v>96</v>
-      </c>
-      <c r="N13">
-        <v>598</v>
-      </c>
       <c r="O13" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="P13" t="s">
         <v>35</v>
       </c>
       <c r="Q13" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="R13" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="F14" t="s">
-        <v>112</v>
+        <v>115</v>
+      </c>
+      <c r="G14" t="s">
+        <v>116</v>
       </c>
       <c r="I14" t="s">
-        <v>100</v>
+        <v>117</v>
+      </c>
+      <c r="J14" t="s">
+        <v>118</v>
+      </c>
+      <c r="K14" t="s">
+        <v>119</v>
+      </c>
+      <c r="L14" t="s">
+        <v>120</v>
       </c>
       <c r="M14" t="s">
-        <v>96</v>
-      </c>
-      <c r="N14">
-        <v>392</v>
+        <v>35</v>
+      </c>
+      <c r="N14" t="s">
+        <v>121</v>
       </c>
       <c r="O14" t="s">
-        <v>106</v>
-      </c>
-      <c r="P14" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>107</v>
-      </c>
-      <c r="R14" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>114</v>
+        <v>124</v>
+      </c>
+      <c r="G15" t="s">
+        <v>125</v>
+      </c>
+      <c r="H15" t="s">
+        <v>126</v>
       </c>
       <c r="I15" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="J15" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="K15" t="s">
-        <v>117</v>
-      </c>
-      <c r="L15">
-        <v>61201021621</v>
+        <v>119</v>
+      </c>
+      <c r="L15" t="s">
+        <v>127</v>
       </c>
       <c r="M15" t="s">
         <v>35</v>
       </c>
       <c r="N15" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="O15" t="s">
-        <v>119</v>
-      </c>
-      <c r="P15" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>120</v>
-      </c>
-      <c r="R15" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="B16">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="F16" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="G16" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="I16" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="J16" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="K16" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="L16" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="M16" t="s">
         <v>35</v>
       </c>
       <c r="N16" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="O16" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -2113,117 +2140,114 @@
         <v>2</v>
       </c>
       <c r="F17" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G17" t="s">
-        <v>133</v>
-      </c>
-      <c r="H17" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="I17" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="J17" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="K17" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="L17" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="M17" t="s">
         <v>35</v>
       </c>
       <c r="N17" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="O17" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B18">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="G18" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="I18" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="J18" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="K18" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="L18" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="M18" t="s">
         <v>35</v>
       </c>
       <c r="N18" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="O18" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G19" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="I19" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="J19" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="K19" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="L19" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="M19" t="s">
         <v>35</v>
       </c>
       <c r="N19" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="O19" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -2233,36 +2257,36 @@
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G20" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="I20" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="J20" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="K20" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="L20" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="M20" t="s">
         <v>35</v>
       </c>
       <c r="N20" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="O20" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -2272,245 +2296,167 @@
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G21" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="I21" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="J21" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="K21" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="L21" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="M21" t="s">
         <v>35</v>
       </c>
       <c r="N21" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="O21" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>7</v>
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F22" t="s">
+        <v>115</v>
+      </c>
+      <c r="G22" t="s">
+        <v>143</v>
+      </c>
+      <c r="I22" t="s">
+        <v>144</v>
+      </c>
+      <c r="J22" t="s">
+        <v>145</v>
+      </c>
+      <c r="K22" t="s">
+        <v>146</v>
+      </c>
+      <c r="L22" t="s">
         <v>147</v>
       </c>
-      <c r="G22" t="s">
-        <v>124</v>
-      </c>
-      <c r="I22" t="s">
-        <v>125</v>
-      </c>
-      <c r="J22" t="s">
-        <v>126</v>
-      </c>
-      <c r="K22" t="s">
-        <v>127</v>
-      </c>
-      <c r="L22" t="s">
-        <v>128</v>
-      </c>
       <c r="M22" t="s">
+        <v>22</v>
+      </c>
+      <c r="N22" t="s">
+        <v>148</v>
+      </c>
+      <c r="O22" t="s">
+        <v>149</v>
+      </c>
+      <c r="P22" t="s">
         <v>35</v>
       </c>
-      <c r="N22" t="s">
-        <v>129</v>
-      </c>
-      <c r="O22" t="s">
-        <v>130</v>
+      <c r="Q22" t="s">
+        <v>150</v>
+      </c>
+      <c r="R22" t="s">
+        <v>151</v>
+      </c>
+      <c r="S22" t="s">
+        <v>24</v>
+      </c>
+      <c r="T22" t="s">
+        <v>152</v>
+      </c>
+      <c r="U22" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E23">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F23" t="s">
-        <v>149</v>
-      </c>
-      <c r="G23" t="s">
-        <v>124</v>
+        <v>155</v>
       </c>
       <c r="I23" t="s">
-        <v>125</v>
+        <v>156</v>
       </c>
       <c r="J23" t="s">
-        <v>126</v>
+        <v>157</v>
       </c>
       <c r="K23" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="L23" t="s">
-        <v>128</v>
+        <v>159</v>
       </c>
       <c r="M23" t="s">
         <v>35</v>
       </c>
       <c r="N23" t="s">
-        <v>129</v>
+        <v>160</v>
       </c>
       <c r="O23" t="s">
-        <v>130</v>
+        <v>161</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="B24">
-        <v>8</v>
-      </c>
-      <c r="C24">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E24">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>123</v>
-      </c>
-      <c r="G24" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="I24" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="J24" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="K24" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="L24" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="M24" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="N24" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="O24" t="s">
-        <v>157</v>
-      </c>
-      <c r="P24" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>158</v>
-      </c>
-      <c r="R24" t="s">
-        <v>159</v>
-      </c>
-      <c r="S24" t="s">
-        <v>24</v>
-      </c>
-      <c r="T24" t="s">
-        <v>160</v>
-      </c>
-      <c r="U24" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>162</v>
-      </c>
-      <c r="B25">
-        <v>2</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F25" t="s">
-        <v>163</v>
-      </c>
-      <c r="I25" t="s">
-        <v>164</v>
-      </c>
-      <c r="J25" t="s">
-        <v>165</v>
-      </c>
-      <c r="K25" t="s">
-        <v>166</v>
-      </c>
-      <c r="L25" t="s">
-        <v>167</v>
-      </c>
-      <c r="M25" t="s">
-        <v>35</v>
-      </c>
-      <c r="N25" t="s">
         <v>168</v>
-      </c>
-      <c r="O25" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>170</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="E26">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F26" t="s">
-        <v>171</v>
-      </c>
-      <c r="I26" t="s">
-        <v>172</v>
-      </c>
-      <c r="J26" t="s">
-        <v>173</v>
-      </c>
-      <c r="K26" t="s">
-        <v>166</v>
-      </c>
-      <c r="L26" t="s">
-        <v>174</v>
-      </c>
-      <c r="M26" t="s">
-        <v>35</v>
-      </c>
-      <c r="N26" t="s">
-        <v>175</v>
-      </c>
-      <c r="O26" t="s">
-        <v>176</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E26">
+  <conditionalFormatting sqref="E2:E24">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Mixer2 - BOM update
</commit_message>
<xml_diff>
--- a/modules/Mixer2/Mixer2-BOM.xlsx
+++ b/modules/Mixer2/Mixer2-BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\Mixer2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA9765C-8E12-4791-926A-6544F91AE98E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A12BE6-CB28-4DB9-BF81-110B63C8E7A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2310" yWindow="1260" windowWidth="19110" windowHeight="10695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4305" yWindow="1155" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mixer2-BOM" sheetId="1" r:id="rId1"/>
@@ -1449,7 +1449,7 @@
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1666,10 +1666,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
@@ -2083,10 +2080,7 @@
         <v>2</v>
       </c>
       <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
@@ -2341,10 +2335,7 @@
         <v>1</v>
       </c>
       <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E21">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Mixer2: update BOM & README
</commit_message>
<xml_diff>
--- a/modules/Mixer2/Mixer2-BOM.xlsx
+++ b/modules/Mixer2/Mixer2-BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\Mixer2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7BFEC8-4134-4A05-972A-6B5E04F7FC1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946E39DE-2EAF-4774-BCBD-6449D3D58AA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="1830" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4635" yWindow="1080" windowWidth="19380" windowHeight="11685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mixer2-BOM" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
             <charset val="1"/>
           </rPr>
           <t>D-shaft for small knobs.
-Also need more knobs!</t>
+Also need the knobs!</t>
         </r>
       </text>
     </comment>
@@ -1449,7 +1449,7 @@
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1852,10 +1852,7 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>6</v>
-      </c>
-      <c r="D10">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
@@ -2377,10 +2374,7 @@
         <v>8</v>
       </c>
       <c r="C22">
-        <v>7</v>
-      </c>
-      <c r="D22">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E22">
         <f t="shared" si="0"/>

</xml_diff>